<commit_message>
Finished to implement scheduleGen, both on back and frontend
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>geogr(marcio)</t>
+          <t>histo(marcio)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -507,7 +507,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -566,7 +566,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -574,17 +578,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7h45</t>
+          <t>13h15</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>geogr(marcio)</t>
+          <t>histo(marcio)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>---(---)</t>
+          <t>histo(evando)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -596,12 +600,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8h30</t>
+          <t>14h00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -618,7 +622,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9h15</t>
+          <t>14h45</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -640,12 +644,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10h15</t>
+          <t>15h45</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>---(---)</t>
+          <t>histo(marcio)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -662,12 +666,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11h00</t>
+          <t>16h30</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>---(---)</t>
+          <t>histo(marcio)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -695,7 +699,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>---(---)</t>
+          <t>histo(marcio)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -798,7 +802,11 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
@@ -806,7 +814,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>7h45</t>
+          <t>13h15</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -828,7 +836,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>8h30</t>
+          <t>14h00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -850,7 +858,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>9h15</t>
+          <t>14h45</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -872,7 +880,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>10h15</t>
+          <t>15h45</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -894,7 +902,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>11h00</t>
+          <t>16h30</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1029,6 +1037,598 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>13h15</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14h00</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14h45</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>15h45</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>16h30</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>7h45</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>8h30</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>9h15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>10h15</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>13h15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>14h00</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>14h45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>15h45</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>16h30</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>7h45</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>8h30</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>9h15</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>10h15</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>13h15</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>14h00</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>14h45</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>15h45</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>16h30</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes and implementations: finished scheduleGen for teachers, admin and students, fully implemented passwordRecover, fixed a bug on htmlMail for admin and teachers
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>352</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>351</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>353</t>
         </is>
       </c>
     </row>
@@ -463,17 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>histo(evando)</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
     </row>
@@ -485,17 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>histo(evando)</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
     </row>
@@ -510,16 +480,6 @@
           <t>geogr(marcio)</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>histo(evando)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -529,17 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>histo(evando)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
     </row>
@@ -554,16 +504,6 @@
           <t>geogr(marcio)</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>histo(evando)</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -572,8 +512,6 @@
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -583,17 +521,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>histo(evando)</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
     </row>
@@ -605,17 +533,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>geogr(marcio)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
@@ -627,17 +545,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
@@ -649,17 +557,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
@@ -671,25 +569,13 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -699,17 +585,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>histo(marcio)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
@@ -721,17 +597,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
@@ -743,17 +609,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
@@ -765,17 +621,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
     </row>
@@ -787,17 +633,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
     </row>
@@ -808,8 +644,6 @@
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -819,17 +653,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>geogr(marcio)</t>
         </is>
       </c>
     </row>
@@ -841,17 +665,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
@@ -863,17 +677,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
@@ -885,17 +689,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
@@ -907,25 +701,13 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>---(---)</t>
+          <t>portu(andrea)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -938,16 +720,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -960,16 +732,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -982,16 +744,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1004,16 +756,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1026,16 +768,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1044,8 +776,6 @@
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1058,16 +788,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1080,16 +800,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1102,16 +812,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1124,16 +824,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1142,16 +832,6 @@
         </is>
       </c>
       <c r="B36" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>
@@ -1160,8 +840,6 @@
     <row r="37">
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1174,16 +852,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1196,16 +864,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1218,16 +876,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1240,16 +888,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1262,16 +900,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1280,8 +908,6 @@
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1294,16 +920,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1316,16 +932,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1338,16 +944,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1360,16 +956,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1378,16 +964,6 @@
         </is>
       </c>
       <c r="B48" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>
@@ -1396,8 +972,6 @@
     <row r="49">
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1410,16 +984,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1432,16 +996,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1454,16 +1008,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1476,16 +1020,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1498,16 +1032,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1516,8 +1040,6 @@
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1530,16 +1052,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1552,16 +1064,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1574,16 +1076,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1596,16 +1088,6 @@
           <t>---(---)</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1614,16 +1096,6 @@
         </is>
       </c>
       <c r="B60" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>---(---)</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>

</xml_diff>

<commit_message>
Fixing date issues and minor bugs
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,16 @@
           <t>351</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>354</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>352</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -458,12 +468,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>histo(evandoss)</t>
+          <t>Matem(Marcio)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>matem(evandro)</t>
+          <t>Geogr(Joyci)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Físic(Edilson)</t>
         </is>
       </c>
     </row>
@@ -475,12 +495,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>histo(evandoss)</t>
+          <t>Matem(Marcio)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>matem(evandro)</t>
+          <t>Geogr(Joyci)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Físic(Edilson)</t>
         </is>
       </c>
     </row>
@@ -492,12 +522,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>histo(evandoss)</t>
+          <t>Matem(Marcio)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>matem(evandro)</t>
+          <t>Geogr(Joyci)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Matem(Evandro)</t>
         </is>
       </c>
     </row>
@@ -514,7 +554,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fisic(evandoss)</t>
+          <t>Geogr(Joyci)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Geogr(Evandro)</t>
         </is>
       </c>
     </row>
@@ -531,19 +581,35 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fisic(evandoss)</t>
+          <t>Físic(Edilson)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Matem(Evandro)</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7h45</t>
+          <t>13h15</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -553,14 +619,24 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>matem(evandro)</t>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Geogr(Evandro)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8h30</t>
+          <t>14h00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -570,14 +646,24 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>fisic(evandoss)</t>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Geogr(Evandro)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9h15</t>
+          <t>14h45</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -588,13 +674,23 @@
       <c r="C10" t="inlineStr">
         <is>
           <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Geogr(Evandro)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10h15</t>
+          <t>15h45</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -603,6 +699,16 @@
         </is>
       </c>
       <c r="C11" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>
@@ -611,7 +717,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11h00</t>
+          <t>16h30</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -620,6 +726,16 @@
         </is>
       </c>
       <c r="C12" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>
@@ -629,6 +745,8 @@
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -646,6 +764,16 @@
           <t>---(---)</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -663,6 +791,16 @@
           <t>---(---)</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -680,6 +818,16 @@
           <t>---(---)</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -697,6 +845,16 @@
           <t>---(---)</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -714,16 +872,32 @@
           <t>---(---)</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>7h45</t>
+          <t>13h15</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -732,6 +906,16 @@
         </is>
       </c>
       <c r="C20" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>
@@ -740,7 +924,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>8h30</t>
+          <t>14h00</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -749,6 +933,16 @@
         </is>
       </c>
       <c r="C21" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>
@@ -757,7 +951,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>9h15</t>
+          <t>14h45</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -766,6 +960,16 @@
         </is>
       </c>
       <c r="C22" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>
@@ -774,7 +978,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>10h15</t>
+          <t>15h45</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -783,6 +987,16 @@
         </is>
       </c>
       <c r="C23" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>
@@ -791,7 +1005,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>11h00</t>
+          <t>16h30</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -800,6 +1014,16 @@
         </is>
       </c>
       <c r="C24" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>
@@ -809,6 +1033,8 @@
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -826,6 +1052,16 @@
           <t>---(---)</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -843,6 +1079,16 @@
           <t>---(---)</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -860,6 +1106,16 @@
           <t>---(---)</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -877,6 +1133,16 @@
           <t>---(---)</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -890,6 +1156,738 @@
         </is>
       </c>
       <c r="C30" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>13h15</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14h00</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14h45</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>15h45</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>16h30</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>7h45</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>8h30</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>9h15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>10h15</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>13h15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>14h00</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>14h45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>15h45</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>16h30</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>7h45</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>8h30</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>9h15</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>10h15</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>INTERVALO</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>13h15</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>14h00</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>14h45</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>15h45</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>16h30</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>---(---)</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
         <is>
           <t>---(---)</t>
         </is>

</xml_diff>